<commit_message>
update the file 第四天计分表
</commit_message>
<xml_diff>
--- a/Docs/计分组/给分表/第四天计分表.xlsx
+++ b/Docs/计分组/给分表/第四天计分表.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\栩海\Desktop\给分表\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\栩海\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14265" windowHeight="14835" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="119">
   <si>
     <t>黄馨仪</t>
   </si>
@@ -565,12 +565,24 @@
     <t>认真设计建模，创意火花闪现。很不错</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>额外情况</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>由于提出精彩的见解并且撰写建议书，记分组对其加三十分。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>由于提出精彩的见解并且撰写建议书，记分组对其加三十分。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -637,6 +649,14 @@
       <color theme="11"/>
       <name val="宋体"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -725,7 +745,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -766,9 +786,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -780,6 +797,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1126,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U36"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="W7" sqref="W6:W7"/>
+    <sheetView tabSelected="1" topLeftCell="L4" workbookViewId="0">
+      <selection activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -1145,10 +1168,12 @@
     <col min="14" max="17" width="11" style="1"/>
     <col min="18" max="18" width="11" style="9"/>
     <col min="19" max="19" width="11" style="6"/>
-    <col min="20" max="16384" width="11" style="1"/>
+    <col min="20" max="21" width="11" style="1"/>
+    <col min="22" max="22" width="36.625" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30" customHeight="1">
+    <row r="1" spans="1:23" ht="30" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
@@ -1209,8 +1234,11 @@
       <c r="U1" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:21">
+      <c r="V1" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1235,7 +1263,7 @@
       <c r="H2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="14" t="s">
         <v>108</v>
       </c>
       <c r="J2" s="8">
@@ -1247,7 +1275,7 @@
       <c r="L2" s="1">
         <v>19</v>
       </c>
-      <c r="M2" s="18" t="s">
+      <c r="M2" s="17" t="s">
         <v>112</v>
       </c>
       <c r="N2" s="1">
@@ -1266,7 +1294,7 @@
       <c r="R2" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="S2" s="14" t="s">
+      <c r="S2" s="18" t="s">
         <v>54</v>
       </c>
       <c r="T2" s="1">
@@ -1277,7 +1305,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:23">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -1302,7 +1330,7 @@
       <c r="H3" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="16"/>
+      <c r="I3" s="15"/>
       <c r="J3" s="8">
         <v>9</v>
       </c>
@@ -1312,7 +1340,7 @@
       <c r="L3" s="1">
         <v>19</v>
       </c>
-      <c r="M3" s="18"/>
+      <c r="M3" s="17"/>
       <c r="N3" s="1">
         <f t="shared" ref="N3:N36" si="0">SUM(L3,K3,J3,G3,F3,E3,C3)</f>
         <v>211</v>
@@ -1329,16 +1357,16 @@
       <c r="R3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="S3" s="14"/>
+      <c r="S3" s="18"/>
       <c r="T3" s="1">
         <v>35</v>
       </c>
       <c r="U3" s="1">
-        <f t="shared" ref="U3:V36" si="1">SUM(T3,O3,N3,B3)</f>
+        <f t="shared" ref="U3:U36" si="1">SUM(T3,O3,N3,B3)</f>
         <v>862</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:23">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1363,7 +1391,7 @@
       <c r="H4" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="16"/>
+      <c r="I4" s="15"/>
       <c r="J4" s="8">
         <v>9</v>
       </c>
@@ -1373,7 +1401,7 @@
       <c r="L4" s="1">
         <v>19</v>
       </c>
-      <c r="M4" s="18"/>
+      <c r="M4" s="17"/>
       <c r="N4" s="1">
         <f t="shared" si="0"/>
         <v>207</v>
@@ -1390,7 +1418,7 @@
       <c r="R4" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="S4" s="14"/>
+      <c r="S4" s="18"/>
       <c r="T4" s="1">
         <v>35</v>
       </c>
@@ -1399,7 +1427,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:23">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -1424,7 +1452,7 @@
       <c r="H5" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="16"/>
+      <c r="I5" s="15"/>
       <c r="J5" s="8">
         <v>9</v>
       </c>
@@ -1434,7 +1462,7 @@
       <c r="L5" s="1">
         <v>19</v>
       </c>
-      <c r="M5" s="18"/>
+      <c r="M5" s="17"/>
       <c r="N5" s="1">
         <f t="shared" si="0"/>
         <v>210</v>
@@ -1451,7 +1479,7 @@
       <c r="R5" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="S5" s="14"/>
+      <c r="S5" s="18"/>
       <c r="T5" s="1">
         <v>60</v>
       </c>
@@ -1460,7 +1488,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:23">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
@@ -1485,7 +1513,7 @@
       <c r="H6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="16"/>
+      <c r="I6" s="15"/>
       <c r="J6" s="8">
         <v>9</v>
       </c>
@@ -1495,7 +1523,7 @@
       <c r="L6" s="1">
         <v>19</v>
       </c>
-      <c r="M6" s="18"/>
+      <c r="M6" s="17"/>
       <c r="N6" s="1">
         <f t="shared" si="0"/>
         <v>209</v>
@@ -1512,7 +1540,7 @@
       <c r="R6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="S6" s="14"/>
+      <c r="S6" s="18"/>
       <c r="T6" s="1">
         <v>80</v>
       </c>
@@ -1520,8 +1548,14 @@
         <f t="shared" si="1"/>
         <v>885</v>
       </c>
-    </row>
-    <row r="7" spans="1:21">
+      <c r="V6" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="W6" s="1">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -1546,7 +1580,7 @@
       <c r="H7" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="16"/>
+      <c r="I7" s="15"/>
       <c r="J7" s="8">
         <v>9</v>
       </c>
@@ -1556,7 +1590,7 @@
       <c r="L7" s="1">
         <v>19</v>
       </c>
-      <c r="M7" s="18"/>
+      <c r="M7" s="17"/>
       <c r="N7" s="1">
         <f t="shared" si="0"/>
         <v>209</v>
@@ -1573,7 +1607,7 @@
       <c r="R7" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="S7" s="14"/>
+      <c r="S7" s="18"/>
       <c r="T7" s="1">
         <v>40</v>
       </c>
@@ -1582,7 +1616,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:23">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -1607,7 +1641,7 @@
       <c r="H8" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I8" s="16"/>
+      <c r="I8" s="15"/>
       <c r="J8" s="8">
         <v>9</v>
       </c>
@@ -1617,7 +1651,7 @@
       <c r="L8" s="1">
         <v>19</v>
       </c>
-      <c r="M8" s="18"/>
+      <c r="M8" s="17"/>
       <c r="N8" s="1">
         <f t="shared" si="0"/>
         <v>210</v>
@@ -1634,7 +1668,7 @@
       <c r="R8" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="S8" s="14"/>
+      <c r="S8" s="18"/>
       <c r="T8" s="1">
         <v>38</v>
       </c>
@@ -1643,7 +1677,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:23">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -1668,7 +1702,7 @@
       <c r="H9" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="16"/>
+      <c r="I9" s="15"/>
       <c r="J9" s="8">
         <v>9</v>
       </c>
@@ -1678,7 +1712,7 @@
       <c r="L9" s="1">
         <v>19</v>
       </c>
-      <c r="M9" s="18"/>
+      <c r="M9" s="17"/>
       <c r="N9" s="1">
         <f t="shared" si="0"/>
         <v>210</v>
@@ -1695,7 +1729,7 @@
       <c r="R9" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="S9" s="14"/>
+      <c r="S9" s="18"/>
       <c r="T9" s="1">
         <v>50</v>
       </c>
@@ -1704,7 +1738,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:23">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
@@ -1729,7 +1763,7 @@
       <c r="H10" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="16"/>
+      <c r="I10" s="15"/>
       <c r="J10" s="8">
         <v>9</v>
       </c>
@@ -1739,7 +1773,7 @@
       <c r="L10" s="1">
         <v>19</v>
       </c>
-      <c r="M10" s="18"/>
+      <c r="M10" s="17"/>
       <c r="N10" s="1">
         <f t="shared" si="0"/>
         <v>211</v>
@@ -1756,7 +1790,7 @@
       <c r="R10" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="S10" s="14"/>
+      <c r="S10" s="18"/>
       <c r="T10" s="1">
         <v>65</v>
       </c>
@@ -1765,7 +1799,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:23">
       <c r="A11" s="7" t="s">
         <v>50</v>
       </c>
@@ -1790,7 +1824,7 @@
       <c r="H11" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I11" s="16"/>
+      <c r="I11" s="15"/>
       <c r="J11" s="8">
         <v>9</v>
       </c>
@@ -1800,7 +1834,7 @@
       <c r="L11" s="1">
         <v>19</v>
       </c>
-      <c r="M11" s="18"/>
+      <c r="M11" s="17"/>
       <c r="N11" s="1">
         <f t="shared" si="0"/>
         <v>208</v>
@@ -1817,7 +1851,7 @@
       <c r="R11" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="S11" s="14"/>
+      <c r="S11" s="18"/>
       <c r="T11" s="1">
         <v>60</v>
       </c>
@@ -1826,7 +1860,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:23">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
@@ -1851,7 +1885,7 @@
       <c r="H12" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I12" s="16"/>
+      <c r="I12" s="15"/>
       <c r="J12" s="8">
         <v>9</v>
       </c>
@@ -1861,7 +1895,7 @@
       <c r="L12" s="1">
         <v>19</v>
       </c>
-      <c r="M12" s="18"/>
+      <c r="M12" s="17"/>
       <c r="N12" s="1">
         <f t="shared" si="0"/>
         <v>210</v>
@@ -1878,7 +1912,7 @@
       <c r="R12" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="S12" s="14"/>
+      <c r="S12" s="18"/>
       <c r="T12" s="1">
         <v>80</v>
       </c>
@@ -1887,7 +1921,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:23">
       <c r="A13" s="10" t="s">
         <v>10</v>
       </c>
@@ -1912,7 +1946,7 @@
       <c r="H13" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I13" s="16"/>
+      <c r="I13" s="15"/>
       <c r="J13" s="8">
         <v>9</v>
       </c>
@@ -1922,7 +1956,7 @@
       <c r="L13" s="1">
         <v>18</v>
       </c>
-      <c r="M13" s="18" t="s">
+      <c r="M13" s="17" t="s">
         <v>115</v>
       </c>
       <c r="N13" s="1">
@@ -1941,7 +1975,7 @@
       <c r="R13" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="S13" s="14"/>
+      <c r="S13" s="18"/>
       <c r="T13" s="1">
         <v>98</v>
       </c>
@@ -1950,7 +1984,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:23">
       <c r="A14" s="10" t="s">
         <v>11</v>
       </c>
@@ -1975,7 +2009,7 @@
       <c r="H14" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I14" s="16"/>
+      <c r="I14" s="15"/>
       <c r="J14" s="8">
         <v>9</v>
       </c>
@@ -1985,7 +2019,7 @@
       <c r="L14" s="1">
         <v>18</v>
       </c>
-      <c r="M14" s="18"/>
+      <c r="M14" s="17"/>
       <c r="N14" s="1">
         <f t="shared" si="0"/>
         <v>200</v>
@@ -2002,7 +2036,7 @@
       <c r="R14" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="S14" s="14"/>
+      <c r="S14" s="18"/>
       <c r="T14" s="1">
         <v>55</v>
       </c>
@@ -2011,7 +2045,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:23">
       <c r="A15" s="10" t="s">
         <v>12</v>
       </c>
@@ -2036,7 +2070,7 @@
       <c r="H15" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I15" s="16"/>
+      <c r="I15" s="15"/>
       <c r="J15" s="8">
         <v>9</v>
       </c>
@@ -2046,7 +2080,7 @@
       <c r="L15" s="1">
         <v>18</v>
       </c>
-      <c r="M15" s="18"/>
+      <c r="M15" s="17"/>
       <c r="N15" s="1">
         <f t="shared" si="0"/>
         <v>211</v>
@@ -2063,7 +2097,7 @@
       <c r="R15" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="S15" s="14"/>
+      <c r="S15" s="18"/>
       <c r="T15" s="1">
         <v>45</v>
       </c>
@@ -2072,7 +2106,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:23">
       <c r="A16" s="10" t="s">
         <v>13</v>
       </c>
@@ -2097,7 +2131,7 @@
       <c r="H16" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I16" s="16"/>
+      <c r="I16" s="15"/>
       <c r="J16" s="8">
         <v>9</v>
       </c>
@@ -2107,7 +2141,7 @@
       <c r="L16" s="1">
         <v>18</v>
       </c>
-      <c r="M16" s="18"/>
+      <c r="M16" s="17"/>
       <c r="N16" s="1">
         <f t="shared" si="0"/>
         <v>204</v>
@@ -2124,7 +2158,7 @@
       <c r="R16" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="S16" s="14"/>
+      <c r="S16" s="18"/>
       <c r="T16" s="1">
         <v>85</v>
       </c>
@@ -2158,7 +2192,7 @@
       <c r="H17" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="16"/>
+      <c r="I17" s="15"/>
       <c r="J17" s="8">
         <v>9</v>
       </c>
@@ -2168,7 +2202,7 @@
       <c r="L17" s="1">
         <v>18</v>
       </c>
-      <c r="M17" s="18"/>
+      <c r="M17" s="17"/>
       <c r="N17" s="1">
         <f t="shared" si="0"/>
         <v>208</v>
@@ -2185,7 +2219,7 @@
       <c r="R17" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="S17" s="14"/>
+      <c r="S17" s="18"/>
       <c r="T17" s="1">
         <v>38</v>
       </c>
@@ -2219,7 +2253,7 @@
       <c r="H18" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I18" s="16"/>
+      <c r="I18" s="15"/>
       <c r="J18" s="8">
         <v>9</v>
       </c>
@@ -2229,7 +2263,7 @@
       <c r="L18" s="1">
         <v>18</v>
       </c>
-      <c r="M18" s="18"/>
+      <c r="M18" s="17"/>
       <c r="N18" s="1">
         <f t="shared" si="0"/>
         <v>209</v>
@@ -2246,7 +2280,7 @@
       <c r="R18" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="S18" s="14"/>
+      <c r="S18" s="18"/>
       <c r="T18" s="1">
         <v>40</v>
       </c>
@@ -2280,7 +2314,7 @@
       <c r="H19" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I19" s="16"/>
+      <c r="I19" s="15"/>
       <c r="J19" s="8">
         <v>9</v>
       </c>
@@ -2290,7 +2324,7 @@
       <c r="L19" s="1">
         <v>18</v>
       </c>
-      <c r="M19" s="18"/>
+      <c r="M19" s="17"/>
       <c r="N19" s="1">
         <f t="shared" si="0"/>
         <v>208</v>
@@ -2307,7 +2341,7 @@
       <c r="R19" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="S19" s="14"/>
+      <c r="S19" s="18"/>
       <c r="T19" s="1">
         <v>45</v>
       </c>
@@ -2341,7 +2375,7 @@
       <c r="H20" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I20" s="16"/>
+      <c r="I20" s="15"/>
       <c r="J20" s="8">
         <v>9</v>
       </c>
@@ -2351,7 +2385,7 @@
       <c r="L20" s="1">
         <v>18</v>
       </c>
-      <c r="M20" s="18"/>
+      <c r="M20" s="17"/>
       <c r="N20" s="1">
         <f t="shared" si="0"/>
         <v>208</v>
@@ -2368,7 +2402,7 @@
       <c r="R20" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="S20" s="14"/>
+      <c r="S20" s="18"/>
       <c r="T20" s="1">
         <v>30</v>
       </c>
@@ -2402,7 +2436,7 @@
       <c r="H21" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I21" s="16"/>
+      <c r="I21" s="15"/>
       <c r="J21" s="8">
         <v>9</v>
       </c>
@@ -2412,7 +2446,7 @@
       <c r="L21" s="1">
         <v>18</v>
       </c>
-      <c r="M21" s="18"/>
+      <c r="M21" s="17"/>
       <c r="N21" s="1">
         <f t="shared" si="0"/>
         <v>203</v>
@@ -2429,7 +2463,7 @@
       <c r="R21" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="S21" s="14"/>
+      <c r="S21" s="18"/>
       <c r="T21" s="1">
         <v>20</v>
       </c>
@@ -2463,7 +2497,7 @@
       <c r="H22" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I22" s="16"/>
+      <c r="I22" s="15"/>
       <c r="J22" s="8">
         <v>9</v>
       </c>
@@ -2473,7 +2507,7 @@
       <c r="L22" s="1">
         <v>19</v>
       </c>
-      <c r="M22" s="18" t="s">
+      <c r="M22" s="17" t="s">
         <v>114</v>
       </c>
       <c r="N22" s="1">
@@ -2492,7 +2526,7 @@
       <c r="R22" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="S22" s="14"/>
+      <c r="S22" s="18"/>
       <c r="T22" s="1">
         <v>20</v>
       </c>
@@ -2526,7 +2560,7 @@
       <c r="H23" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I23" s="16"/>
+      <c r="I23" s="15"/>
       <c r="J23" s="8">
         <v>9</v>
       </c>
@@ -2536,7 +2570,7 @@
       <c r="L23" s="1">
         <v>19</v>
       </c>
-      <c r="M23" s="18"/>
+      <c r="M23" s="17"/>
       <c r="N23" s="1">
         <f t="shared" si="0"/>
         <v>208</v>
@@ -2553,7 +2587,7 @@
       <c r="R23" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="S23" s="14"/>
+      <c r="S23" s="18"/>
       <c r="T23" s="1">
         <v>93</v>
       </c>
@@ -2587,7 +2621,7 @@
       <c r="H24" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I24" s="16"/>
+      <c r="I24" s="15"/>
       <c r="J24" s="8">
         <v>9</v>
       </c>
@@ -2597,7 +2631,7 @@
       <c r="L24" s="1">
         <v>19</v>
       </c>
-      <c r="M24" s="18"/>
+      <c r="M24" s="17"/>
       <c r="N24" s="1">
         <f t="shared" si="0"/>
         <v>210</v>
@@ -2614,7 +2648,7 @@
       <c r="R24" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="S24" s="14"/>
+      <c r="S24" s="18"/>
       <c r="T24" s="1">
         <v>38</v>
       </c>
@@ -2648,7 +2682,7 @@
       <c r="H25" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I25" s="16"/>
+      <c r="I25" s="15"/>
       <c r="J25" s="8">
         <v>9</v>
       </c>
@@ -2658,7 +2692,7 @@
       <c r="L25" s="1">
         <v>19</v>
       </c>
-      <c r="M25" s="18"/>
+      <c r="M25" s="17"/>
       <c r="N25" s="1">
         <f t="shared" si="0"/>
         <v>212</v>
@@ -2675,7 +2709,7 @@
       <c r="R25" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="S25" s="14"/>
+      <c r="S25" s="18"/>
       <c r="T25" s="1">
         <v>45</v>
       </c>
@@ -2709,7 +2743,7 @@
       <c r="H26" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I26" s="16"/>
+      <c r="I26" s="15"/>
       <c r="J26" s="8">
         <v>9</v>
       </c>
@@ -2719,7 +2753,7 @@
       <c r="L26" s="1">
         <v>19</v>
       </c>
-      <c r="M26" s="18"/>
+      <c r="M26" s="17"/>
       <c r="N26" s="1">
         <f t="shared" si="0"/>
         <v>208</v>
@@ -2736,7 +2770,7 @@
       <c r="R26" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="S26" s="14"/>
+      <c r="S26" s="18"/>
       <c r="T26" s="1">
         <v>30</v>
       </c>
@@ -2770,7 +2804,7 @@
       <c r="H27" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I27" s="16"/>
+      <c r="I27" s="15"/>
       <c r="J27" s="8">
         <v>9</v>
       </c>
@@ -2780,7 +2814,7 @@
       <c r="L27" s="1">
         <v>19</v>
       </c>
-      <c r="M27" s="18"/>
+      <c r="M27" s="17"/>
       <c r="N27" s="1">
         <f t="shared" si="0"/>
         <v>212</v>
@@ -2797,7 +2831,7 @@
       <c r="R27" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="S27" s="14"/>
+      <c r="S27" s="18"/>
       <c r="T27" s="1">
         <v>50</v>
       </c>
@@ -2831,7 +2865,7 @@
       <c r="H28" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I28" s="16"/>
+      <c r="I28" s="15"/>
       <c r="J28" s="8">
         <v>9</v>
       </c>
@@ -2841,7 +2875,7 @@
       <c r="L28" s="1">
         <v>19</v>
       </c>
-      <c r="M28" s="18"/>
+      <c r="M28" s="17"/>
       <c r="N28" s="1">
         <f t="shared" si="0"/>
         <v>208</v>
@@ -2858,7 +2892,7 @@
       <c r="R28" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="S28" s="14"/>
+      <c r="S28" s="18"/>
       <c r="T28" s="1">
         <v>43</v>
       </c>
@@ -2892,7 +2926,7 @@
       <c r="H29" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I29" s="16"/>
+      <c r="I29" s="15"/>
       <c r="J29" s="8">
         <v>9</v>
       </c>
@@ -2902,7 +2936,7 @@
       <c r="L29" s="1">
         <v>19</v>
       </c>
-      <c r="M29" s="18"/>
+      <c r="M29" s="17"/>
       <c r="N29" s="1">
         <f t="shared" si="0"/>
         <v>210</v>
@@ -2919,7 +2953,7 @@
       <c r="R29" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="S29" s="14"/>
+      <c r="S29" s="18"/>
       <c r="T29" s="1">
         <v>45</v>
       </c>
@@ -2953,7 +2987,7 @@
       <c r="H30" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I30" s="16"/>
+      <c r="I30" s="15"/>
       <c r="J30" s="8">
         <v>9</v>
       </c>
@@ -2963,7 +2997,7 @@
       <c r="L30" s="1">
         <v>19</v>
       </c>
-      <c r="M30" s="18"/>
+      <c r="M30" s="17"/>
       <c r="N30" s="1">
         <f t="shared" si="0"/>
         <v>209</v>
@@ -2980,7 +3014,7 @@
       <c r="R30" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="S30" s="14"/>
+      <c r="S30" s="18"/>
       <c r="T30" s="1">
         <v>10</v>
       </c>
@@ -3014,7 +3048,7 @@
       <c r="H31" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I31" s="16"/>
+      <c r="I31" s="15"/>
       <c r="J31" s="8">
         <v>9</v>
       </c>
@@ -3024,7 +3058,7 @@
       <c r="L31" s="1">
         <v>19</v>
       </c>
-      <c r="M31" s="18"/>
+      <c r="M31" s="17"/>
       <c r="N31" s="1">
         <f t="shared" si="0"/>
         <v>205</v>
@@ -3041,7 +3075,7 @@
       <c r="R31" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="S31" s="14"/>
+      <c r="S31" s="18"/>
       <c r="T31" s="1">
         <v>30</v>
       </c>
@@ -3075,7 +3109,7 @@
       <c r="H32" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I32" s="16"/>
+      <c r="I32" s="15"/>
       <c r="J32" s="8">
         <v>9</v>
       </c>
@@ -3085,7 +3119,7 @@
       <c r="L32" s="1">
         <v>19</v>
       </c>
-      <c r="M32" s="18"/>
+      <c r="M32" s="17"/>
       <c r="N32" s="1">
         <f t="shared" si="0"/>
         <v>211</v>
@@ -3102,7 +3136,7 @@
       <c r="R32" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="S32" s="14"/>
+      <c r="S32" s="18"/>
       <c r="T32" s="1">
         <v>48</v>
       </c>
@@ -3111,7 +3145,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:23">
       <c r="A33" s="10" t="s">
         <v>30</v>
       </c>
@@ -3136,7 +3170,7 @@
       <c r="H33" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I33" s="16"/>
+      <c r="I33" s="15"/>
       <c r="J33" s="8">
         <v>9</v>
       </c>
@@ -3146,7 +3180,7 @@
       <c r="L33" s="1">
         <v>18</v>
       </c>
-      <c r="M33" s="18" t="s">
+      <c r="M33" s="17" t="s">
         <v>113</v>
       </c>
       <c r="N33" s="1">
@@ -3165,7 +3199,7 @@
       <c r="R33" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="S33" s="14"/>
+      <c r="S33" s="18"/>
       <c r="T33" s="1">
         <v>18</v>
       </c>
@@ -3174,7 +3208,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:23">
       <c r="A34" s="10" t="s">
         <v>31</v>
       </c>
@@ -3199,7 +3233,7 @@
       <c r="H34" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I34" s="16"/>
+      <c r="I34" s="15"/>
       <c r="J34" s="8">
         <v>9</v>
       </c>
@@ -3209,7 +3243,7 @@
       <c r="L34" s="1">
         <v>18</v>
       </c>
-      <c r="M34" s="18"/>
+      <c r="M34" s="17"/>
       <c r="N34" s="1">
         <f t="shared" si="0"/>
         <v>208</v>
@@ -3226,7 +3260,7 @@
       <c r="R34" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="S34" s="14"/>
+      <c r="S34" s="18"/>
       <c r="T34" s="1">
         <v>143</v>
       </c>
@@ -3234,8 +3268,14 @@
         <f t="shared" si="1"/>
         <v>914</v>
       </c>
-    </row>
-    <row r="35" spans="1:21">
+      <c r="V34" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="W34" s="1">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23">
       <c r="A35" s="10" t="s">
         <v>32</v>
       </c>
@@ -3260,7 +3300,7 @@
       <c r="H35" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I35" s="16"/>
+      <c r="I35" s="15"/>
       <c r="J35" s="8">
         <v>9</v>
       </c>
@@ -3270,7 +3310,7 @@
       <c r="L35" s="1">
         <v>18</v>
       </c>
-      <c r="M35" s="18"/>
+      <c r="M35" s="17"/>
       <c r="N35" s="1">
         <f t="shared" si="0"/>
         <v>207</v>
@@ -3287,7 +3327,7 @@
       <c r="R35" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="S35" s="14"/>
+      <c r="S35" s="18"/>
       <c r="T35" s="1">
         <v>23</v>
       </c>
@@ -3296,7 +3336,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="36" spans="1:21">
+    <row r="36" spans="1:23">
       <c r="A36" s="10" t="s">
         <v>33</v>
       </c>
@@ -3321,7 +3361,7 @@
       <c r="H36" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I36" s="17"/>
+      <c r="I36" s="16"/>
       <c r="J36" s="8">
         <v>9</v>
       </c>
@@ -3331,7 +3371,7 @@
       <c r="L36" s="1">
         <v>18</v>
       </c>
-      <c r="M36" s="18"/>
+      <c r="M36" s="17"/>
       <c r="N36" s="1">
         <f t="shared" si="0"/>
         <v>207</v>
@@ -3348,7 +3388,7 @@
       <c r="R36" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="S36" s="14"/>
+      <c r="S36" s="18"/>
       <c r="T36" s="1">
         <v>23</v>
       </c>
@@ -3368,7 +3408,7 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="R24 R35:R36" twoDigitTextYear="1"/>
   </ignoredErrors>

</xml_diff>